<commit_message>
added some sql commenting (not finished yet) and a test
</commit_message>
<xml_diff>
--- a/DataTakeOnTesting.xlsx
+++ b/DataTakeOnTesting.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>Test name</t>
   </si>
@@ -205,6 +205,27 @@
   </si>
   <si>
     <t>Correct data and Roomno count of 84</t>
+  </si>
+  <si>
+    <t>Checking to see if all of the values inside of a column are unique (for the purpose of validating primary keys)</t>
+  </si>
+  <si>
+    <t>Run a script that checks each value and counts how many identical values are inside of the column, the script then returns the count of each value that it found</t>
+  </si>
+  <si>
+    <t>SELECT PCID, COUNT(PCID) 
+FROM PCALLOCATION
+GROUP BY PCID
+HAVING COUNT(PCID) &gt; 1;</t>
+  </si>
+  <si>
+    <t>For the purpose of primary keys, the expected result of this test would be for every value to be unique(no value having COUNT &gt; 1). For the purpose of this test, the PCALLOCATION table will be used for the PCID column</t>
+  </si>
+  <si>
+    <t>No value having COUNT &gt; 1</t>
+  </si>
+  <si>
+    <t>Checks to see that every value used for a column is unique</t>
   </si>
 </sst>
 </file>
@@ -567,11 +588,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,6 +839,26 @@
       </c>
       <c r="F13" s="1" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More progress on testing, fixed error in event data
</commit_message>
<xml_diff>
--- a/DataTakeOnTesting.xlsx
+++ b/DataTakeOnTesting.xlsx
@@ -590,9 +590,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>